<commit_message>
making server proccess data sequencially and give user more control on data received
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:I5"/>
+  <dimension ref="B2:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,7 +589,874 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dfdrsgf</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LKIHJ</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nbvfght</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sdfwe</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CGFDER</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>gyuynfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>asdkhe</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>XCVHOER</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>etjklc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>cxmxm</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>WERERWERE</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>yuyuyuyuyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>skjdfhj</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SKFLEIO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>rotkkdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>THERE</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>how</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>castron</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>VAGAS</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>jose</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>KAMAU</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>gachau</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>mitchelle</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>KAMAU</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>gachau</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>KAMAU</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>gachau</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>michelle</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>KAMAU</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>gachau</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>castron</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>JOSEPH</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>vagas</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>castron</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>VAGAS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nancy</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>MTOTO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>what</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>yy</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>YY</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>castron</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>VAGAS</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>hellp</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>mitchelle</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>KAMAU</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>beatrice</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>MONENTO</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>utel</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>beatrice</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>CHAPAULINGE</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>rafiki</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>rose</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>NDAUKA</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>actress</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>steve</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>NYERERE</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>team leader</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>nadya</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TL</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>utel</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding dropdown list for selection
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:I37"/>
+  <dimension ref="B2:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1427,7 +1427,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
           <t>nadya</t>
@@ -1453,8 +1452,90 @@
           <t>utel</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>EGIFRID ANGELO MWOLEKA</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_happinesa</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>HAPPINES ANDREA KIJAZI</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>192.168.0.250</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>4:55</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Mycc issue/ drop calls</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>EGIFRID ANGELO MWOLEKA</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abuum</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>ABUU MOHAMMED SHAMTE</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>192.168.0.250</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>8:45</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Mycc issue/ drop calls</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Adding general issue report page
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:I39"/>
+  <dimension ref="B2:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1537,7 +1537,1280 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdalaha</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>ABDALLAH MOHAMEDI NGAONA</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Mycc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adamm</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>ADAM RAMADHANI MSONGE</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>12:01</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Mycc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CASTRON JOSEPH VAGAS</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>ABDULHALIM OMAR BAKAR</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CASTRON JOSEPH VAGAS</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>ABDULHALIM OMAR BAKAR</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CASTRON JOSEPH VAGAS</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>ABDULHALIM OMAR BAKAR</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CASTRON JOSEPH VAGAS</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ABDULHALIM OMAR BAKAR</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CASTRON JOSEPH VAGAS</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ABDULHALIM OMAR BAKAR</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_agnessp</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>AGNESS PATRICK NDELWA</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>12:23</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_agnessp</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>AGNESS PATRICK NDELWA</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>12:23</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>DANIEL OTIENO MUSSA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdalaha</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>ABDALAH ATHUMANI</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>DANIEL OTIENO MUSSA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdalaha</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ABDALAH ATHUMANI</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>DANIEL OTIENO MUSSA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdalaha</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ABDALAH ATHUMANI</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>DANIEL OTIENO MUSSA</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdalaha</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>ABDALAH ATHUMANI</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Power cut</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>WALES ELIAS LETAWO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adolphcm</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>ADOLPH CLEMENCE MALIBICHE</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>EGIFRID ANGELO MWOLEKA</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adamm</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>ADAM RAMADHANI MSONGE</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Pc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_zulfah</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>ZULFA HUSSEIN</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>192.168.169.154</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>20:08</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>hello there friend how are you?</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>There was a power outage between 3:00am to 3:05am which affected some agents for 5min</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_adamm</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>ABDALLAH MOHAMEDI NGAONA</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>06:35</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Mycc issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>HAMISI MRISHO SHABANI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>halotel_ut_cc_abdulhalimob</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>ABDALLAH RAMADHANI YUSUPH</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>07:19</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Mycc issue</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B69:I69"/>
+    <mergeCell ref="B71:I71"/>
+    <mergeCell ref="B70:I70"/>
+  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>